<commit_message>
Create df for emissions
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/Temporary_ToHelpBuildDecks/TMP_ExistingCapacity_UniqueTechNameLv2.xlsx
+++ b/CreateBaseDeck/ExcelUserData/Temporary_ToHelpBuildDecks/TMP_ExistingCapacity_UniqueTechNameLv2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NG_CA_Existing</t>
+          <t>NG_CC_Existing</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,226 +496,202 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NG_CT_Existing</t>
+          <t>BLQ_ST_Existing</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Natural Gas Fired Combined Cycle</t>
+          <t>Wood/Wood Waste Biomass</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BLQ_ST_Existing</t>
+          <t>SUN_PV_Existing</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Wood/Wood Waste Biomass</t>
+          <t>Solar Photovoltaic</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SUN_PV_Existing</t>
+          <t>MWH_BA1h_Existing</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Solar Photovoltaic</t>
+          <t>Batteries</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MWH_BA1h_Existing</t>
+          <t>DFO_GT_Existing</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Batteries</t>
+          <t>Petroleum Liquids</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DFO_GT_Existing</t>
+          <t>WDS_ST_Existing</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Petroleum Liquids</t>
+          <t>Wood/Wood Waste Biomass</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>WDS_ST_Existing</t>
+          <t>WH_ST_Existing</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Wood/Wood Waste Biomass</t>
+          <t>All Other</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>WH_ST_Existing</t>
+          <t>LFG_IC_Existing</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>All Other</t>
+          <t>Landfill Gas</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LFG_IC_Existing</t>
+          <t>WND_WT_Existing</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Landfill Gas</t>
+          <t>Onshore Wind Turbine</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>WND_WT_Existing</t>
+          <t>AB_ST_Existing</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Onshore Wind Turbine</t>
+          <t>Other Waste Biomass</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AB_ST_Existing</t>
+          <t>NG_ST_Existing</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Other Waste Biomass</t>
+          <t>Natural Gas Steam Turbine</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NG_ST_Existing</t>
+          <t>WAT_HY_Existing</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Natural Gas Steam Turbine</t>
+          <t>Conventional Hydroelectric</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>WAT_HY_Existing</t>
+          <t>WAT_PS_Existing</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Conventional Hydroelectric</t>
+          <t>Hydroelectric Pumped Storage</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WAT_PS_Existing</t>
+          <t>DFO_CC_Existing</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hydroelectric Pumped Storage</t>
+          <t>Petroleum Liquids</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DFO_CT_Existing</t>
+          <t>BIT_ST_Existing</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Petroleum Liquids</t>
+          <t>Conventional Steam Coal</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DFO_CA_Existing</t>
+          <t>LFG_GT_Existing</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Petroleum Liquids</t>
+          <t>Landfill Gas</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BIT_ST_Existing</t>
+          <t>OBG_IC_Existing</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Conventional Steam Coal</t>
+          <t>Other Waste Biomass</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LFG_GT_Existing</t>
+          <t>MWH_BA2h_Existing</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
-        <is>
-          <t>Landfill Gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>OBG_IC_Existing</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Other Waste Biomass</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>MWH_BA2h_Existing</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
         <is>
           <t>Batteries</t>
         </is>

</xml_diff>